<commit_message>
Add: Filter option "auth_level_request"
</commit_message>
<xml_diff>
--- a/tests/px2/standard/px-files/sitemaps/sitemap.xlsx
+++ b/tests/px2/standard/px-files/sitemaps/sitemap.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.9-alpha.1%2Bnb</t>
   </si>
@@ -23,7 +23,7 @@
     <t>「Pickles 2 Practice 1」 サイトマップ</t>
   </si>
   <si>
-    <t>Exported: 2018-03-28 15:00:29</t>
+    <t>Exported: 2018-03-31 18:54:47</t>
   </si>
   <si>
     <t>ページID</t>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>/sample2/</t>
+  </si>
+  <si>
+    <t>My Page</t>
+  </si>
+  <si>
+    <t>/mypage/</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>/admin/</t>
   </si>
   <si>
     <t>Logout</t>
@@ -637,7 +649,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
@@ -935,36 +947,98 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="15" spans="1:21" customHeight="1" ht="5">
-      <c r="A15" s="10" t="s">
+    <row r="13" spans="1:21">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="4">
+        <v>1</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+    </row>
+    <row r="17" spans="1:21" customHeight="1" ht="5">
+      <c r="A17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>